<commit_message>
update templates with second 'Logging' timesheet
</commit_message>
<xml_diff>
--- a/data/templates/template_timesheet_19_days.xlsx
+++ b/data/templates/template_timesheet_19_days.xlsx
@@ -5,10 +5,11 @@
   <workbookPr backupFile="false" showObjects="all" date1904="true"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Tabelle1" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Logging" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Timesheet" sheetId="2" state="visible" r:id="rId3"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -20,7 +21,16 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="23">
+  <si>
+    <t xml:space="preserve">carryover</t>
+  </si>
+  <si>
+    <t xml:space="preserve">row</t>
+  </si>
+  <si>
+    <t xml:space="preserve">column</t>
+  </si>
   <si>
     <t xml:space="preserve">Stundenzettel</t>
   </si>
@@ -502,9 +512,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>153360</xdr:colOff>
+      <xdr:colOff>152640</xdr:colOff>
       <xdr:row>4</xdr:row>
-      <xdr:rowOff>192240</xdr:rowOff>
+      <xdr:rowOff>191520</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -518,7 +528,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="332280" y="178200"/>
-          <a:ext cx="2477160" cy="1116360"/>
+          <a:ext cx="2476440" cy="1115640"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -536,12 +546,60 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B8" activeCellId="0" sqref="B8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="11.4"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B1" s="0" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="0" t="n">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="0" t="n">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="true"/>
   </sheetPr>
   <dimension ref="A1:M1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D12" activeCellId="0" sqref="D12:G30"/>
+      <selection pane="topLeft" activeCell="J32" activeCellId="0" sqref="J32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.65" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -620,7 +678,7 @@
     <row r="5" customFormat="false" ht="21.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1"/>
       <c r="B5" s="2" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C5" s="2"/>
       <c r="D5" s="2"/>
@@ -653,7 +711,7 @@
       <c r="A7" s="1"/>
       <c r="B7" s="3"/>
       <c r="C7" s="4" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D7" s="5"/>
       <c r="E7" s="5"/>
@@ -670,14 +728,14 @@
       <c r="A8" s="1"/>
       <c r="B8" s="3"/>
       <c r="C8" s="4" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="D8" s="5"/>
       <c r="E8" s="5"/>
       <c r="F8" s="5"/>
       <c r="G8" s="5"/>
       <c r="H8" s="7" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="I8" s="7"/>
       <c r="J8" s="8" t="n">
@@ -706,32 +764,32 @@
       <c r="A10" s="1"/>
       <c r="B10" s="3"/>
       <c r="C10" s="4" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="F10" s="4" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="G10" s="4" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="H10" s="4" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="I10" s="4" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="J10" s="4" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="K10" s="4"/>
       <c r="L10" s="9" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="M10" s="1"/>
     </row>
@@ -1230,7 +1288,7 @@
       <c r="F32" s="6"/>
       <c r="G32" s="6"/>
       <c r="H32" s="7" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="I32" s="7"/>
       <c r="J32" s="27" t="n">
@@ -1290,7 +1348,7 @@
       <c r="A36" s="1"/>
       <c r="B36" s="3"/>
       <c r="C36" s="28" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="D36" s="29" t="n">
         <f aca="false">ROWS(D12:D30)*8</f>
@@ -1300,7 +1358,7 @@
       <c r="F36" s="3"/>
       <c r="G36" s="3"/>
       <c r="H36" s="30" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="I36" s="29" t="n">
         <f aca="false">SUM(I12:I30)</f>
@@ -1345,19 +1403,19 @@
       <c r="A39" s="1"/>
       <c r="B39" s="1"/>
       <c r="C39" s="1" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="D39" s="1"/>
       <c r="E39" s="1"/>
       <c r="F39" s="1"/>
       <c r="G39" s="1" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="H39" s="1"/>
       <c r="I39" s="1"/>
       <c r="J39" s="1"/>
       <c r="K39" s="1" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="L39" s="1"/>
       <c r="M39" s="1"/>
@@ -1381,19 +1439,19 @@
       <c r="A41" s="1"/>
       <c r="B41" s="1"/>
       <c r="C41" s="1" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="D41" s="1"/>
       <c r="E41" s="1"/>
       <c r="F41" s="1"/>
       <c r="G41" s="1" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="H41" s="1"/>
       <c r="I41" s="1"/>
       <c r="J41" s="1"/>
       <c r="K41" s="1" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="L41" s="1"/>
       <c r="M41" s="1"/>

</xml_diff>